<commit_message>
Adição de dummy html
</commit_message>
<xml_diff>
--- a/media/planilhas/planilha.xlsx
+++ b/media/planilhas/planilha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Área de Trabalho\Pedro\Cursos\Django\Pegasus\static\exemplo_planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078FB541-F3C6-47DB-B83F-AA578EB07CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30ECC99-5951-4E0E-A27D-E6BBE61D7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83751D9D-0AA3-4700-A02B-38810A7D263F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>